<commit_message>
Change the `Method` column into `Type`
</commit_message>
<xml_diff>
--- a/data-raw/biovolume_method.xlsx
+++ b/data-raw/biovolume_method.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tumha\Desktop\Lab Work\R_packages\GRSmacrofauna\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tumha\Desktop\Lab Work\R_packages\GRSmacrofauna\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A62175D-380B-464B-8599-10AA0DEDF91F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272D9AF9-D290-47DC-AB4E-17625BA271DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{C19946F7-BC32-4ACF-B65E-5A4C5E50E524}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{C19946F7-BC32-4ACF-B65E-5A4C5E50E524}"/>
   </bookViews>
   <sheets>
     <sheet name="biovolume_method" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>Taxon</t>
   </si>
@@ -186,16 +186,13 @@
     <t>Scleractinia</t>
   </si>
   <si>
-    <t xml:space="preserve">Although all bryozoans are colonial, solitary specimen might occur due to sample processing </t>
-  </si>
-  <si>
-    <t>Both arms and discs were assumed to be cylindrical</t>
-  </si>
-  <si>
     <t>Priapulida</t>
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Both arms and discs are assumed to be cylindrical</t>
   </si>
 </sst>
 </file>
@@ -557,8 +554,8 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -578,7 +575,7 @@
         <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -672,9 +669,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
@@ -993,7 +988,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1056,17 +1051,15 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.53</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">

</xml_diff>